<commit_message>
added BNN and more overlap
</commit_message>
<xml_diff>
--- a/data/test_data/date_test.xlsx
+++ b/data/test_data/date_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDocuments\Disertatie\segments\data\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4986641-072D-4D27-82F6-8232B6BBC7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0385B586-C039-4EE2-9030-AB458BB07DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{3B65094A-8F75-4249-ACCD-01D821DD3F26}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{3B65094A-8F75-4249-ACCD-01D821DD3F26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,41 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Pozitie</t>
+  </si>
+  <si>
+    <t>Severitate def</t>
+  </si>
+  <si>
+    <t>Mod 2</t>
+  </si>
+  <si>
+    <t>Mod 3</t>
+  </si>
+  <si>
+    <t>Mod 4</t>
+  </si>
+  <si>
+    <t>Mod 5</t>
+  </si>
+  <si>
+    <t>Mod 6</t>
+  </si>
+  <si>
+    <t>Mod 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mod1 </t>
+  </si>
+  <si>
+    <t>Mod 8</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,8 +101,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,47 +420,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBDBD44-1EEB-4194-8D29-BEA9AC8711F5}">
-  <dimension ref="A1:J315"/>
+  <dimension ref="A1:K313"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
+      <selection activeCell="A298" sqref="A298:XFD298"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="B1">
-        <v>12</v>
-      </c>
-      <c r="C1">
-        <v>1.1328397346722402E-3</v>
-      </c>
-      <c r="D1">
-        <v>9.949555757394102E-4</v>
-      </c>
-      <c r="E1">
-        <v>8.7838361990356907E-4</v>
-      </c>
-      <c r="F1">
-        <v>7.6640022445139614E-4</v>
-      </c>
-      <c r="G1">
-        <v>6.623470852785984E-4</v>
-      </c>
-      <c r="H1">
-        <v>5.6602760916264142E-4</v>
-      </c>
-      <c r="I1">
-        <v>4.7748291830113635E-4</v>
-      </c>
-      <c r="J1">
-        <v>3.96726366916264E-4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>2.7E-2</v>
       </c>
@@ -454,7 +493,7 @@
         <v>1.6287640855224927E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -486,7 +525,7 @@
         <v>4.1917100954890882E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>7.1999999999999995E-2</v>
       </c>
@@ -518,7 +557,7 @@
         <v>2.5983804556467364E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>0.09</v>
       </c>
@@ -550,7 +589,7 @@
         <v>4.6914808839524931E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>9.9000000000000005E-2</v>
       </c>
@@ -582,7 +621,7 @@
         <v>5.1633051599378466E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>0.11700000000000001</v>
       </c>
@@ -614,7 +653,7 @@
         <v>4.5696716816983951E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>0.126</v>
       </c>
@@ -646,7 +685,7 @@
         <v>3.6404472083535403E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>0.153</v>
       </c>
@@ -678,7 +717,7 @@
         <v>5.2623643742646348E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>0.18</v>
       </c>
@@ -710,7 +749,7 @@
         <v>6.0678790300666859E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>0.19800000000000001</v>
       </c>
@@ -742,7 +781,7 @@
         <v>2.751237999932786E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>0.22500000000000001</v>
       </c>
@@ -774,7 +813,7 @@
         <v>5.7702445961692198E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>0.26100000000000001</v>
       </c>
@@ -806,7 +845,7 @@
         <v>3.7779097768524084E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>0.27900000000000003</v>
       </c>
@@ -838,7 +877,7 @@
         <v>1.3485279474113087E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>0.29699999999999999</v>
       </c>
@@ -870,7 +909,7 @@
         <v>3.0254163406591046E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>0.33300000000000002</v>
       </c>
@@ -902,7 +941,7 @@
         <v>2.9287490255680641E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>0.35099999999999998</v>
       </c>
@@ -934,7 +973,7 @@
         <v>5.1783242091798241E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>0.378</v>
       </c>
@@ -966,7 +1005,7 @@
         <v>5.5398866468587909E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>0.39600000000000002</v>
       </c>
@@ -998,7 +1037,7 @@
         <v>3.535256723213307E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>0.41399999999999998</v>
       </c>
@@ -1030,7 +1069,7 @@
         <v>1.1524894760270478E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>0.432</v>
       </c>
@@ -1062,7 +1101,7 @@
         <v>5.8665897111707283E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>0.441</v>
       </c>
@@ -1094,7 +1133,7 @@
         <v>1.922797920009922E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>0.46800000000000003</v>
       </c>
@@ -1126,7 +1165,7 @@
         <v>3.1648901702942825E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>0.48599999999999999</v>
       </c>
@@ -1158,7 +1197,7 @@
         <v>5.3308258509736567E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>0.495</v>
       </c>
@@ -1190,7 +1229,7 @@
         <v>5.8734069523880717E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>0.52200000000000002</v>
       </c>
@@ -1222,7 +1261,7 @@
         <v>4.4936183264721405E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>0.55800000000000005</v>
       </c>
@@ -1254,7 +1293,7 @@
         <v>2.4486645309760349E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>0.57599999999999996</v>
       </c>
@@ -1286,7 +1325,7 @@
         <v>2.8348992223606677E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>0.60299999999999998</v>
       </c>
@@ -1318,7 +1357,7 @@
         <v>3.3979592672453489E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>0.621</v>
       </c>
@@ -1350,7 +1389,7 @@
         <v>5.4677944118730853E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>0.64800000000000002</v>
       </c>
@@ -1382,7 +1421,7 @@
         <v>5.2742787545974248E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>0.67500000000000004</v>
       </c>
@@ -1414,7 +1453,7 @@
         <v>1.8404810392627091E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>0.68400000000000005</v>
       </c>
@@ -1446,7 +1485,7 @@
         <v>8.0890075778633619E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>0.69299999999999995</v>
       </c>
@@ -1478,7 +1517,7 @@
         <v>1.6154996676813622E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>0.72</v>
       </c>
@@ -1510,7 +1549,7 @@
         <v>1.2222945885447241E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>0.747</v>
       </c>
@@ -1542,7 +1581,7 @@
         <v>4.7463890595745472E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>0.78300000000000003</v>
       </c>
@@ -1574,7 +1613,7 @@
         <v>5.0694253926478433E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>0.81</v>
       </c>
@@ -1606,7 +1645,7 @@
         <v>1.5762776853288189E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>0.83699999999999997</v>
       </c>
@@ -1638,7 +1677,7 @@
         <v>6.1326337041359291E-6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>0.873</v>
       </c>
@@ -1670,7 +1709,7 @@
         <v>4.2008165499041921E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>0.90900000000000003</v>
       </c>
@@ -1702,7 +1741,7 @@
         <v>6.6974882385739817E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>0.92700000000000005</v>
       </c>
@@ -1734,7 +1773,7 @@
         <v>5.1620542454089825E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>0.94499999999999995</v>
       </c>
@@ -1766,7 +1805,7 @@
         <v>2.7711091783943093E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>0.98099999999999998</v>
       </c>
@@ -1798,7 +1837,7 @@
         <v>8.6596233623158263E-6</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>0.999</v>
       </c>
@@ -1830,7 +1869,7 @@
         <v>9.0168002884699981E-11</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -1862,7 +1901,7 @@
         <v>7.1308876539863961E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>2.7E-2</v>
       </c>
@@ -1894,7 +1933,7 @@
         <v>2.9275930911746624E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -1926,7 +1965,7 @@
         <v>7.5343148985411927E-7</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>7.1999999999999995E-2</v>
       </c>
@@ -1958,7 +1997,7 @@
         <v>4.6704128227105399E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>0.09</v>
       </c>
@@ -1990,7 +2029,7 @@
         <v>8.4326190301717849E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>9.9000000000000005E-2</v>
       </c>
@@ -2022,7 +2061,7 @@
         <v>9.2806911990642464E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>0.11700000000000001</v>
       </c>
@@ -2054,7 +2093,7 @@
         <v>8.2136752419765787E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>0.126</v>
       </c>
@@ -2086,7 +2125,7 @@
         <v>6.5434572082567755E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>0.153</v>
       </c>
@@ -2118,7 +2157,7 @@
         <v>9.4587434253246651E-5</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>0.18</v>
       </c>
@@ -2150,7 +2189,7 @@
         <v>1.0906601443638917E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>0.19800000000000001</v>
       </c>
@@ -2182,7 +2221,7 @@
         <v>4.9451639021108498E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>0.22500000000000001</v>
       </c>
@@ -2214,7 +2253,7 @@
         <v>1.0371623714132818E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>0.26100000000000001</v>
       </c>
@@ -2246,7 +2285,7 @@
         <v>6.7905368617250141E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>0.27900000000000003</v>
       </c>
@@ -2278,7 +2317,7 @@
         <v>2.4238876195694308E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>0.29699999999999999</v>
       </c>
@@ -2310,7 +2349,7 @@
         <v>5.4379808933466367E-6</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>0.33300000000000002</v>
       </c>
@@ -2342,7 +2381,7 @@
         <v>5.2642279439057429E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>0.35099999999999998</v>
       </c>
@@ -2374,7 +2413,7 @@
         <v>9.3076869225012094E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>0.378</v>
       </c>
@@ -2406,7 +2445,7 @@
         <v>9.9575709075337346E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>0.39600000000000002</v>
       </c>
@@ -2438,7 +2477,7 @@
         <v>6.3543844381170364E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>0.41399999999999998</v>
       </c>
@@ -2470,7 +2509,7 @@
         <v>2.0715217493182486E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>0.432</v>
       </c>
@@ -2502,7 +2541,7 @@
         <v>1.0544797530742581E-6</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>0.441</v>
       </c>
@@ -2534,7 +2573,7 @@
         <v>3.456098987190199E-5</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>0.46800000000000003</v>
       </c>
@@ -2566,7 +2605,7 @@
         <v>5.6886756524397752E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>0.48599999999999999</v>
       </c>
@@ -2598,7 +2637,7 @@
         <v>9.5817982912849815E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>0.495</v>
       </c>
@@ -2630,7 +2669,7 @@
         <v>1.0557051059946821E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>0.52200000000000002</v>
       </c>
@@ -2662,7 +2701,7 @@
         <v>8.0769744887489495E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>0.55800000000000005</v>
       </c>
@@ -2694,7 +2733,7 @@
         <v>4.4013085917167878E-5</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>0.57599999999999996</v>
       </c>
@@ -2726,7 +2765,7 @@
         <v>5.0955392811827203E-5</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>0.60299999999999998</v>
       </c>
@@ -2758,7 +2797,7 @@
         <v>6.1076015632363504E-4</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>0.621</v>
       </c>
@@ -2790,7 +2829,7 @@
         <v>9.8279899995633909E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>0.64800000000000002</v>
       </c>
@@ -2822,7 +2861,7 @@
         <v>9.4801587167459001E-4</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>0.67500000000000004</v>
       </c>
@@ -2854,7 +2893,7 @@
         <v>3.3081399712070583E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>0.68400000000000005</v>
       </c>
@@ -2886,7 +2925,7 @@
         <v>1.4539443072147254E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>0.69299999999999995</v>
       </c>
@@ -2918,7 +2957,7 @@
         <v>2.9037511988003653E-5</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>0.72</v>
       </c>
@@ -2950,7 +2989,7 @@
         <v>2.1969917096101727E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>0.747</v>
       </c>
@@ -2982,7 +3021,7 @@
         <v>8.5313127556959213E-4</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>0.78300000000000003</v>
       </c>
@@ -3014,7 +3053,7 @@
         <v>9.1119486779328736E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>0.81</v>
       </c>
@@ -3046,7 +3085,7 @@
         <v>2.8332523429021241E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>0.83699999999999997</v>
       </c>
@@ -3078,7 +3117,7 @@
         <v>1.1022993582998724E-5</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>0.873</v>
       </c>
@@ -3110,7 +3149,7 @@
         <v>7.5506831333688922E-4</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>0.90900000000000003</v>
       </c>
@@ -3142,7 +3181,7 @@
         <v>1.2038281338443702E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>0.92700000000000005</v>
       </c>
@@ -3174,7 +3213,7 @@
         <v>9.2784427649509791E-4</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>0.94499999999999995</v>
       </c>
@@ -3206,7 +3245,7 @@
         <v>4.9808809990769165E-4</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>0.98099999999999998</v>
       </c>
@@ -3238,7 +3277,7 @@
         <v>1.556508628415506E-5</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>0.999</v>
       </c>
@@ -3270,7 +3309,7 @@
         <v>1.6207087609350362E-10</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -3302,7 +3341,7 @@
         <v>1.1144294959638419E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>2.7E-2</v>
       </c>
@@ -3334,7 +3373,7 @@
         <v>4.5753014930211504E-4</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -3366,7 +3405,7 @@
         <v>1.1774779189124138E-6</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>7.1999999999999995E-2</v>
       </c>
@@ -3398,7 +3437,7 @@
         <v>7.2990152986728018E-4</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>0.09</v>
       </c>
@@ -3430,7 +3469,7 @@
         <v>1.3178666992735336E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>9.9000000000000005E-2</v>
       </c>
@@ -3462,7 +3501,7 @@
         <v>1.4504051272477057E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>0.11700000000000001</v>
       </c>
@@ -3494,7 +3533,7 @@
         <v>1.2836497227395681E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>0.126</v>
       </c>
@@ -3526,7 +3565,7 @@
         <v>1.0226246818489672E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>0.153</v>
       </c>
@@ -3558,7 +3597,7 @@
         <v>1.4782314880592816E-4</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>0.18</v>
       </c>
@@ -3590,7 +3629,7 @@
         <v>1.7045056575415535E-4</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>0.19800000000000001</v>
       </c>
@@ -3622,7 +3661,7 @@
         <v>7.7284018235894284E-4</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>0.22500000000000001</v>
       </c>
@@ -3654,7 +3693,7 @@
         <v>1.6208982596445931E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>0.26100000000000001</v>
       </c>
@@ -3686,7 +3725,7 @@
         <v>1.0612387881199583E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>0.27900000000000003</v>
       </c>
@@ -3718,7 +3757,7 @@
         <v>3.7881004290393923E-4</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>0.29699999999999999</v>
       </c>
@@ -3750,7 +3789,7 @@
         <v>8.4985861509757796E-6</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>0.33300000000000002</v>
       </c>
@@ -3782,7 +3821,7 @@
         <v>8.2270415393320966E-4</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>0.35099999999999998</v>
       </c>
@@ -3814,7 +3853,7 @@
         <v>1.4546240733204594E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>0.378</v>
       </c>
@@ -3846,7 +3885,7 @@
         <v>1.5561892524422886E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>0.39600000000000002</v>
       </c>
@@ -3878,7 +3917,7 @@
         <v>9.9307600822633288E-4</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>0.41399999999999998</v>
       </c>
@@ -3910,7 +3949,7 @@
         <v>3.2374159445357545E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>0.432</v>
       </c>
@@ -3942,7 +3981,7 @@
         <v>1.6479622127627812E-6</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>0.441</v>
       </c>
@@ -3974,7 +4013,7 @@
         <v>5.4012611601619634E-5</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>0.46800000000000003</v>
       </c>
@@ -4006,7 +4045,7 @@
         <v>8.8903769736242894E-4</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>0.48599999999999999</v>
       </c>
@@ -4038,7 +4077,7 @@
         <v>1.4974627505475345E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>0.495</v>
       </c>
@@ -4070,7 +4109,7 @@
         <v>1.6498772190056891E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>0.52200000000000002</v>
       </c>
@@ -4102,7 +4141,7 @@
         <v>1.2622858534837988E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>0.55800000000000005</v>
       </c>
@@ -4134,7 +4173,7 @@
         <v>6.8784537822668437E-5</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>0.57599999999999996</v>
       </c>
@@ -4166,7 +4205,7 @@
         <v>7.9634114970495787E-5</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>0.60299999999999998</v>
       </c>
@@ -4198,7 +4237,7 @@
         <v>9.5450828311120718E-4</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>0.621</v>
       </c>
@@ -4230,7 +4269,7 @@
         <v>1.5359380869544694E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>0.64800000000000002</v>
       </c>
@@ -4262,7 +4301,7 @@
         <v>1.4815783129683998E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>0.67500000000000004</v>
       </c>
@@ -4294,7 +4333,7 @@
         <v>5.1700278276423865E-4</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>0.68400000000000005</v>
       </c>
@@ -4326,7 +4365,7 @@
         <v>2.2722534697948768E-4</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>0.69299999999999995</v>
       </c>
@@ -4358,7 +4397,7 @@
         <v>4.5380409030486547E-5</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>0.72</v>
       </c>
@@ -4390,7 +4429,7 @@
         <v>3.4335029275196533E-4</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>0.747</v>
       </c>
@@ -4422,7 +4461,7 @@
         <v>1.3332907536308016E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>0.78300000000000003</v>
       </c>
@@ -4454,7 +4493,7 @@
         <v>1.424033705918837E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>0.81</v>
       </c>
@@ -4486,7 +4525,7 @@
         <v>4.4278638700382083E-4</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>0.83699999999999997</v>
       </c>
@@ -4518,7 +4557,7 @@
         <v>1.7226956556869305E-5</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>0.873</v>
       </c>
@@ -4550,7 +4589,7 @@
         <v>1.1800359796439769E-3</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>0.90900000000000003</v>
       </c>
@@ -4582,7 +4621,7 @@
         <v>1.8813668725762163E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>0.92700000000000005</v>
       </c>
@@ -4614,7 +4653,7 @@
         <v>1.45005373743242E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>0.94499999999999995</v>
       </c>
@@ -4646,7 +4685,7 @@
         <v>7.7842212226609218E-4</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>0.98099999999999998</v>
       </c>
@@ -4678,7 +4717,7 @@
         <v>2.4325430583088141E-5</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>0.999</v>
       </c>
@@ -4710,7 +4749,7 @@
         <v>2.5328763194625713E-10</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -4742,7 +4781,7 @@
         <v>1.7066083624157396E-3</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>2.7E-2</v>
       </c>
@@ -4774,7 +4813,7 @@
         <v>7.0064977792156855E-4</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -4806,7 +4845,7 @@
         <v>1.8031590784824367E-6</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>7.1999999999999995E-2</v>
       </c>
@@ -4838,7 +4877,7 @@
         <v>1.1177522302873056E-3</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>0.09</v>
       </c>
@@ -4870,7 +4909,7 @@
         <v>2.0181468075593841E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>9.9000000000000005E-2</v>
       </c>
@@ -4902,7 +4941,7 @@
         <v>2.2211127110475463E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>0.11700000000000001</v>
       </c>
@@ -4934,7 +4973,7 @@
         <v>1.9657478191074996E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>0.126</v>
       </c>
@@ -4966,7 +5005,7 @@
         <v>1.5660208563905481E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>0.153</v>
       </c>
@@ -4998,7 +5037,7 @@
         <v>2.2637252766953726E-4</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>0.18</v>
       </c>
@@ -5030,7 +5069,7 @@
         <v>2.6102356582275311E-4</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>0.19800000000000001</v>
       </c>
@@ -5062,7 +5101,7 @@
         <v>1.1835073665956437E-3</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>0.22500000000000001</v>
       </c>
@@ -5094,7 +5133,7 @@
         <v>2.4822014623205315E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>0.26100000000000001</v>
       </c>
@@ -5126,7 +5165,7 @@
         <v>1.6251534950257893E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>0.27900000000000003</v>
       </c>
@@ -5158,7 +5197,7 @@
         <v>5.8009985317896068E-4</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>0.29699999999999999</v>
       </c>
@@ -5190,7 +5229,7 @@
         <v>1.3014513925281496E-5</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>0.33300000000000002</v>
       </c>
@@ -5222,7 +5261,7 @@
         <v>1.2598677565351663E-3</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>0.35099999999999998</v>
       </c>
@@ -5254,7 +5293,7 @@
         <v>2.2275734953990187E-3</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>0.378</v>
       </c>
@@ -5286,7 +5325,7 @@
         <v>2.3831077706917376E-3</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>0.39600000000000002</v>
       </c>
@@ -5318,7 +5357,7 @@
         <v>1.5207707856724655E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>0.41399999999999998</v>
       </c>
@@ -5350,7 +5389,7 @@
         <v>4.957694626329264E-4</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>0.432</v>
       </c>
@@ -5382,7 +5421,7 @@
         <v>2.5236464966441977E-6</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>0.441</v>
       </c>
@@ -5414,7 +5453,7 @@
         <v>8.271350944055435E-5</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>0.46800000000000003</v>
       </c>
@@ -5446,7 +5485,7 @@
         <v>1.3614492207147954E-3</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>0.48599999999999999</v>
       </c>
@@ -5478,7 +5517,7 @@
         <v>2.293175532185855E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>0.495</v>
       </c>
@@ -5510,7 +5549,7 @@
         <v>2.5265790874272501E-3</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>0.52200000000000002</v>
       </c>
@@ -5542,7 +5581,7 @@
         <v>1.9330317450467363E-3</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>0.55800000000000005</v>
       </c>
@@ -5574,7 +5613,7 @@
         <v>1.0533485328431795E-4</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>0.57599999999999996</v>
       </c>
@@ -5606,7 +5645,7 @@
         <v>1.2194961371215718E-4</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>0.60299999999999998</v>
       </c>
@@ -5638,7 +5677,7 @@
         <v>1.4617091739337175E-3</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>0.621</v>
       </c>
@@ -5670,7 +5709,7 @@
         <v>2.3520956622583673E-3</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>0.64800000000000002</v>
       </c>
@@ -5702,7 +5741,7 @@
         <v>2.2688505173661631E-3</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>0.67500000000000004</v>
       </c>
@@ -5734,7 +5773,7 @@
         <v>7.9172462291529752E-4</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>0.68400000000000005</v>
       </c>
@@ -5766,7 +5805,7 @@
         <v>3.4796699002714979E-4</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>0.69299999999999995</v>
       </c>
@@ -5798,7 +5837,7 @@
         <v>6.9494378802576013E-5</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>0.72</v>
       </c>
@@ -5830,7 +5869,7 @@
         <v>5.2579771351224912E-4</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>0.747</v>
       </c>
@@ -5862,7 +5901,7 @@
         <v>2.04176680347999E-3</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>0.78300000000000003</v>
       </c>
@@ -5894,7 +5933,7 @@
         <v>2.1807282019048555E-3</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>0.81</v>
       </c>
@@ -5926,7 +5965,7 @@
         <v>6.7807156357703804E-4</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>0.83699999999999997</v>
       </c>
@@ -5958,7 +5997,7 @@
         <v>2.6380913485692323E-5</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>0.873</v>
       </c>
@@ -5990,7 +6029,7 @@
         <v>1.8070764261943054E-3</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>0.90900000000000003</v>
       </c>
@@ -6022,7 +6061,7 @@
         <v>2.8810763257245053E-3</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>0.92700000000000005</v>
       </c>
@@ -6054,7 +6093,7 @@
         <v>2.2205746018181998E-3</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>0.94499999999999995</v>
       </c>
@@ -6086,7 +6125,7 @@
         <v>1.1920554042763982E-3</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>0.98099999999999998</v>
       </c>
@@ -6118,7 +6157,7 @@
         <v>3.7251332096659383E-5</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>0.999</v>
       </c>
@@ -6150,7 +6189,7 @@
         <v>3.8787809578039683E-10</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -6182,7 +6221,7 @@
         <v>2.3663838303058173E-3</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>2.7E-2</v>
       </c>
@@ -6214,7 +6253,7 @@
         <v>9.7152125917982694E-4</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -6246,7 +6285,7 @@
         <v>2.5002610913906436E-6</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>7.1999999999999995E-2</v>
       </c>
@@ -6278,7 +6317,7 @@
         <v>1.5498756845982217E-3</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>0.09</v>
       </c>
@@ -6310,7 +6349,7 @@
         <v>2.7983631615584705E-3</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>9.9000000000000005E-2</v>
       </c>
@@ -6342,7 +6381,7 @@
         <v>3.0797957636101384E-3</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>0.11700000000000001</v>
       </c>
@@ -6374,7 +6413,7 @@
         <v>2.7257067034467796E-3</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>0.126</v>
       </c>
@@ -6406,7 +6445,7 @@
         <v>2.1714451388475651E-3</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>0.153</v>
       </c>
@@ -6438,7 +6477,7 @@
         <v>3.1388823639910972E-4</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>0.18</v>
       </c>
@@ -6470,7 +6509,7 @@
         <v>3.6193537960718035E-4</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>0.19800000000000001</v>
       </c>
@@ -6502,7 +6541,7 @@
         <v>1.6410517826101572E-3</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>0.22500000000000001</v>
       </c>
@@ -6534,7 +6573,7 @@
         <v>3.4418215293883924E-3</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>0.26100000000000001</v>
       </c>
@@ -6566,7 +6605,7 @@
         <v>2.2534384789667222E-3</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>0.27900000000000003</v>
       </c>
@@ -6598,7 +6637,7 @@
         <v>8.0436668585306286E-4</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>0.29699999999999999</v>
       </c>
@@ -6630,7 +6669,7 @@
         <v>1.8045930156161754E-5</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>0.33300000000000002</v>
       </c>
@@ -6662,7 +6701,7 @@
         <v>1.7469331295015735E-3</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>0.35099999999999998</v>
       </c>
@@ -6694,7 +6733,7 @@
         <v>3.0887542897471932E-3</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>0.378</v>
       </c>
@@ -6726,7 +6765,7 @@
         <v>3.3044181773833909E-3</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>0.39600000000000002</v>
       </c>
@@ -6758,7 +6797,7 @@
         <v>2.10870137289303E-3</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>0.41399999999999998</v>
       </c>
@@ -6790,7 +6829,7 @@
         <v>6.8743413296844464E-4</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>0.432</v>
       </c>
@@ -6822,7 +6861,7 @@
         <v>3.4992892303735011E-6</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>0.441</v>
       </c>
@@ -6854,7 +6893,7 @@
         <v>1.1469058490426756E-4</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>0.46800000000000003</v>
       </c>
@@ -6886,7 +6925,7 @@
         <v>1.8877860279095013E-3</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>0.48599999999999999</v>
       </c>
@@ -6918,7 +6957,7 @@
         <v>3.1797180999020617E-3</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>0.495</v>
       </c>
@@ -6950,7 +6989,7 @@
         <v>3.5033555619131489E-3</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>0.52200000000000002</v>
       </c>
@@ -6982,7 +7021,7 @@
         <v>2.6803425822146004E-3</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>0.55800000000000005</v>
       </c>
@@ -7014,7 +7053,7 @@
         <v>1.4605734922499097E-4</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>0.57599999999999996</v>
       </c>
@@ -7046,7 +7085,7 @@
         <v>1.6909538260553167E-4</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>0.60299999999999998</v>
       </c>
@@ -7078,7 +7117,7 @@
         <v>2.026806518696642E-3</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>0.621</v>
       </c>
@@ -7110,7 +7149,7 @@
         <v>3.2614167755640896E-3</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>0.64800000000000002</v>
       </c>
@@ -7142,7 +7181,7 @@
         <v>3.1459890247322979E-3</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>0.67500000000000004</v>
       </c>
@@ -7174,7 +7213,7 @@
         <v>1.0978056752691157E-3</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>0.68400000000000005</v>
       </c>
@@ -7206,7 +7245,7 @@
         <v>4.8249116599596392E-4</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>0.69299999999999995</v>
       </c>
@@ -7238,7 +7277,7 @@
         <v>9.6360933133352467E-5</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>0.72</v>
       </c>
@@ -7270,7 +7309,7 @@
         <v>7.290713175141779E-4</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>0.747</v>
       </c>
@@ -7302,7 +7341,7 @@
         <v>2.8311146572439199E-3</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>0.78300000000000003</v>
       </c>
@@ -7334,7 +7373,7 @@
         <v>3.0237985872604185E-3</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>0.81</v>
       </c>
@@ -7366,7 +7405,7 @@
         <v>9.4021429823979818E-4</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>0.83699999999999997</v>
       </c>
@@ -7398,7 +7437,7 @@
         <v>3.6579785073168018E-5</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>0.873</v>
       </c>
@@ -7430,7 +7469,7 @@
         <v>2.5056928872772698E-3</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>0.90900000000000003</v>
       </c>
@@ -7462,7 +7501,7 @@
         <v>3.9949015727432178E-3</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>0.92700000000000005</v>
       </c>
@@ -7494,7 +7533,7 @@
         <v>3.079049621139899E-3</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>0.94499999999999995</v>
       </c>
@@ -7526,7 +7565,7 @@
         <v>1.6529044950391229E-3</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>0.98099999999999998</v>
       </c>
@@ -7558,7 +7597,7 @@
         <v>5.1652711818490896E-5</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>0.999</v>
       </c>
@@ -7590,7 +7629,7 @@
         <v>5.3783192101864559E-10</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -7622,7 +7661,7 @@
         <v>3.169789745398111E-3</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>2.7E-2</v>
       </c>
@@ -7654,7 +7693,7 @@
         <v>1.3013603648510804E-3</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -7686,7 +7725,7 @@
         <v>3.3491193891752263E-6</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>7.1999999999999995E-2</v>
       </c>
@@ -7718,7 +7757,7 @@
         <v>2.0760706647688768E-3</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>0.09</v>
       </c>
@@ -7750,7 +7789,7 @@
         <v>3.7484294558679187E-3</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>9.9000000000000005E-2</v>
       </c>
@@ -7782,7 +7821,7 @@
         <v>4.125410638962294E-3</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>0.11700000000000001</v>
       </c>
@@ -7814,7 +7853,7 @@
         <v>3.651105558996285E-3</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>0.126</v>
       </c>
@@ -7846,7 +7885,7 @@
         <v>2.9086678355658255E-3</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>0.153</v>
       </c>
@@ -7878,7 +7917,7 @@
         <v>4.2045576047162792E-4</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>0.18</v>
       </c>
@@ -7910,7 +7949,7 @@
         <v>4.848152865494132E-4</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A236">
         <v>0.19800000000000001</v>
       </c>
@@ -7942,7 +7981,7 @@
         <v>2.1982017648898141E-3</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A237">
         <v>0.22500000000000001</v>
       </c>
@@ -7974,7 +8013,7 @@
         <v>4.6103469984984831E-3</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A238">
         <v>0.26100000000000001</v>
       </c>
@@ -8006,7 +8045,7 @@
         <v>3.0184985592937911E-3</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A239">
         <v>0.27900000000000003</v>
       </c>
@@ -8038,7 +8077,7 @@
         <v>1.0774554996969353E-3</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A240">
         <v>0.29699999999999999</v>
       </c>
@@ -8070,7 +8109,7 @@
         <v>2.4172665322759425E-5</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A241">
         <v>0.33300000000000002</v>
       </c>
@@ -8102,7 +8141,7 @@
         <v>2.3400306614986869E-3</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A242">
         <v>0.35099999999999998</v>
       </c>
@@ -8134,7 +8173,7 @@
         <v>4.1374106551555446E-3</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A243">
         <v>0.378</v>
       </c>
@@ -8166,7 +8205,7 @@
         <v>4.426294128211378E-3</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A244">
         <v>0.39600000000000002</v>
       </c>
@@ -8198,7 +8237,7 @@
         <v>2.8246220677730994E-3</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A245">
         <v>0.41399999999999998</v>
       </c>
@@ -8230,7 +8269,7 @@
         <v>9.2082342577468231E-4</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A246">
         <v>0.432</v>
       </c>
@@ -8262,7 +8301,7 @@
         <v>4.6873254357838071E-6</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A247">
         <v>0.441</v>
       </c>
@@ -8294,7 +8333,7 @@
         <v>1.5362894018603748E-4</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A248">
         <v>0.46800000000000003</v>
       </c>
@@ -8326,7 +8365,7 @@
         <v>2.5287042263131285E-3</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A249">
         <v>0.48599999999999999</v>
       </c>
@@ -8358,7 +8397,7 @@
         <v>4.2592573940229157E-3</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A250">
         <v>0.495</v>
       </c>
@@ -8390,7 +8429,7 @@
         <v>4.6927723188509981E-3</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A251">
         <v>0.52200000000000002</v>
       </c>
@@ -8422,7 +8461,7 @@
         <v>3.5903399619493449E-3</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A252">
         <v>0.55800000000000005</v>
       </c>
@@ -8454,7 +8493,7 @@
         <v>1.9564496760171636E-4</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A253">
         <v>0.57599999999999996</v>
       </c>
@@ -8486,7 +8525,7 @@
         <v>2.2650459444185575E-4</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A254">
         <v>0.60299999999999998</v>
       </c>
@@ -8518,7 +8557,7 @@
         <v>2.7149232667129869E-3</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A255">
         <v>0.621</v>
       </c>
@@ -8550,7 +8589,7 @@
         <v>4.3686934123938811E-3</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A256">
         <v>0.64800000000000002</v>
       </c>
@@ -8582,7 +8621,7 @@
         <v>4.2140770326522655E-3</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A257">
         <v>0.67500000000000004</v>
       </c>
@@ -8614,7 +8653,7 @@
         <v>1.4705193330611039E-3</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A258">
         <v>0.68400000000000005</v>
       </c>
@@ -8646,7 +8685,7 @@
         <v>6.4630071023665425E-4</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A259">
         <v>0.69299999999999995</v>
       </c>
@@ -8678,7 +8717,7 @@
         <v>1.290762275296734E-4</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A260">
         <v>0.72</v>
       </c>
@@ -8710,7 +8749,7 @@
         <v>9.7659676182864676E-4</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A261">
         <v>0.747</v>
       </c>
@@ -8742,7 +8781,7 @@
         <v>3.7923003418335196E-3</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A262">
         <v>0.78300000000000003</v>
       </c>
@@ -8774,7 +8813,7 @@
         <v>4.0504019809874574E-3</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A263">
         <v>0.81</v>
       </c>
@@ -8806,7 +8845,7 @@
         <v>1.259424444534021E-3</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A264">
         <v>0.83699999999999997</v>
       </c>
@@ -8838,7 +8877,7 @@
         <v>4.8998909698774501E-5</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A265">
         <v>0.873</v>
       </c>
@@ -8870,7 +8909,7 @@
         <v>3.3563953224705861E-3</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A266">
         <v>0.90900000000000003</v>
       </c>
@@ -8902,7 +8941,7 @@
         <v>5.3512020649328675E-3</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A267">
         <v>0.92700000000000005</v>
       </c>
@@ -8934,1539 +8973,1475 @@
         <v>4.1244111752571748E-3</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A268">
-        <v>0.94499999999999995</v>
+        <v>0.98099999999999998</v>
       </c>
       <c r="B268">
         <v>32</v>
       </c>
       <c r="C268">
-        <v>2.5573647982261571E-7</v>
+        <v>3.7666371244245102E-9</v>
       </c>
       <c r="D268">
-        <v>8.7990181553893148E-6</v>
+        <v>1.4156550126677546E-7</v>
       </c>
       <c r="E268">
-        <v>6.0753659673508573E-5</v>
+        <v>1.0658733685817897E-6</v>
       </c>
       <c r="F268">
-        <v>2.0303842660785121E-4</v>
+        <v>3.9231302314347005E-6</v>
       </c>
       <c r="G268">
-        <v>4.7843506962312403E-4</v>
+        <v>1.0267058723646903E-5</v>
       </c>
       <c r="H268">
-        <v>9.1107170448071699E-4</v>
+        <v>2.1921551067500431E-5</v>
       </c>
       <c r="I268">
-        <v>1.4993843273692722E-3</v>
+        <v>4.0876696485626469E-5</v>
       </c>
       <c r="J268">
-        <v>2.2140785663754096E-3</v>
-      </c>
-    </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.9189213578718965E-5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A269">
-        <v>0.98099999999999998</v>
+        <v>0.999</v>
       </c>
       <c r="B269">
         <v>32</v>
       </c>
       <c r="C269">
-        <v>3.7666371244245102E-9</v>
+        <v>2.9390467421098671E-14</v>
       </c>
       <c r="D269">
-        <v>1.4156550126677546E-7</v>
+        <v>1.1516219902119809E-12</v>
       </c>
       <c r="E269">
-        <v>1.0658733685817897E-6</v>
+        <v>9.0114037085237188E-12</v>
       </c>
       <c r="F269">
-        <v>3.9231302314347005E-6</v>
+        <v>3.4532872842429435E-11</v>
       </c>
       <c r="G269">
-        <v>1.0267058723646903E-5</v>
+        <v>9.415299891382219E-11</v>
       </c>
       <c r="H269">
-        <v>2.1921551067500431E-5</v>
+        <v>2.0966422774097727E-10</v>
       </c>
       <c r="I269">
-        <v>4.0876696485626469E-5</v>
+        <v>4.080560953325475E-10</v>
       </c>
       <c r="J269">
-        <v>6.9189213578718965E-5</v>
-      </c>
-    </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.2043008668308448E-10</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A270">
-        <v>0.999</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="B270">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C270">
-        <v>2.9390467421098671E-14</v>
+        <v>1.1825935420563184E-2</v>
       </c>
       <c r="D270">
-        <v>1.1516219902119809E-12</v>
+        <v>1.0386535733960475E-2</v>
       </c>
       <c r="E270">
-        <v>9.0114037085237188E-12</v>
+        <v>9.1696183012732659E-3</v>
       </c>
       <c r="F270">
-        <v>3.4532872842429435E-11</v>
+        <v>8.0006017473333198E-3</v>
       </c>
       <c r="G270">
-        <v>9.415299891382219E-11</v>
+        <v>6.9143706887799207E-3</v>
       </c>
       <c r="H270">
-        <v>2.0966422774097727E-10</v>
+        <v>5.9088728505359723E-3</v>
       </c>
       <c r="I270">
-        <v>4.080560953325475E-10</v>
+        <v>4.9845375152602813E-3</v>
       </c>
       <c r="J270">
-        <v>7.2043008668308448E-10</v>
-      </c>
-    </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4.1415040902884736E-3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A271">
-        <v>1.7999999999999999E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="B271">
         <v>36</v>
       </c>
       <c r="C271">
-        <v>1.1825935420563184E-2</v>
+        <v>1.1527392244670937E-2</v>
       </c>
       <c r="D271">
-        <v>1.0386535733960475E-2</v>
+        <v>9.4317793932804737E-3</v>
       </c>
       <c r="E271">
-        <v>9.1696183012732659E-3</v>
+        <v>7.7243845474694716E-3</v>
       </c>
       <c r="F271">
-        <v>8.0006017473333198E-3</v>
+        <v>6.1524886217961972E-3</v>
       </c>
       <c r="G271">
-        <v>6.9143706887799207E-3</v>
+        <v>4.7661632830335986E-3</v>
       </c>
       <c r="H271">
-        <v>5.9088728505359723E-3</v>
+        <v>3.5625611310795171E-3</v>
       </c>
       <c r="I271">
-        <v>4.9845375152602813E-3</v>
+        <v>2.5412735851501013E-3</v>
       </c>
       <c r="J271">
-        <v>4.1415040902884736E-3</v>
-      </c>
-    </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.7002986654855059E-3</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A272">
-        <v>2.7E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="B272">
         <v>36</v>
       </c>
       <c r="C272">
-        <v>1.1527392244670937E-2</v>
+        <v>1.0941788026807751E-2</v>
       </c>
       <c r="D272">
-        <v>9.4317793932804737E-3</v>
+        <v>7.6613521082561573E-3</v>
       </c>
       <c r="E272">
-        <v>7.7243845474694716E-3</v>
+        <v>5.2118572210887075E-3</v>
       </c>
       <c r="F272">
-        <v>6.1524886217961972E-3</v>
+        <v>3.2017519821666766E-3</v>
       </c>
       <c r="G272">
-        <v>4.7661632830335986E-3</v>
+        <v>1.7003065218968E-3</v>
       </c>
       <c r="H272">
-        <v>3.5625611310795171E-3</v>
+        <v>6.8856623773837244E-4</v>
       </c>
       <c r="I272">
-        <v>2.5412735851501013E-3</v>
+        <v>1.3799166519493051E-4</v>
       </c>
       <c r="J272">
-        <v>1.7002986654855059E-3</v>
-      </c>
-    </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4.3758081018687807E-6</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A273">
-        <v>4.4999999999999998E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="B273">
         <v>36</v>
       </c>
       <c r="C273">
-        <v>1.0941788026807751E-2</v>
+        <v>1.0092199730524913E-2</v>
       </c>
       <c r="D273">
-        <v>7.6613521082561573E-3</v>
+        <v>5.3557402694834966E-3</v>
       </c>
       <c r="E273">
-        <v>5.2118572210887075E-3</v>
+        <v>2.3928599692316964E-3</v>
       </c>
       <c r="F273">
-        <v>3.2017519821666766E-3</v>
+        <v>6.1322949708501255E-4</v>
       </c>
       <c r="G273">
-        <v>1.7003065218968E-3</v>
+        <v>3.9274984971421042E-6</v>
       </c>
       <c r="H273">
-        <v>6.8856623773837244E-4</v>
+        <v>3.550281058088721E-4</v>
       </c>
       <c r="I273">
-        <v>1.3799166519493051E-4</v>
+        <v>1.3735720081062726E-3</v>
       </c>
       <c r="J273">
-        <v>4.3758081018687807E-6</v>
-      </c>
-    </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.7125001468475437E-3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A274">
-        <v>7.1999999999999995E-2</v>
+        <v>0.09</v>
       </c>
       <c r="B274">
         <v>36</v>
       </c>
       <c r="C274">
-        <v>1.0092199730524913E-2</v>
+        <v>9.5451353991280238E-3</v>
       </c>
       <c r="D274">
-        <v>5.3557402694834966E-3</v>
+        <v>4.0533420091295033E-3</v>
       </c>
       <c r="E274">
-        <v>2.3928599692316964E-3</v>
+        <v>1.1382655524311352E-3</v>
       </c>
       <c r="F274">
-        <v>6.1322949708501255E-4</v>
+        <v>2.239570483782532E-5</v>
       </c>
       <c r="G274">
-        <v>3.9274984971421042E-6</v>
+        <v>4.5261404599521648E-4</v>
       </c>
       <c r="H274">
-        <v>3.550281058088721E-4</v>
+        <v>1.8574846916962426E-3</v>
       </c>
       <c r="I274">
-        <v>1.3735720081062726E-3</v>
+        <v>3.5541932981112455E-3</v>
       </c>
       <c r="J274">
-        <v>2.7125001468475437E-3</v>
-      </c>
-    </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4.8975285967066641E-3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A275">
-        <v>0.09</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="B275">
         <v>36</v>
       </c>
       <c r="C275">
-        <v>9.5451353991280238E-3</v>
+        <v>9.2774371460456629E-3</v>
       </c>
       <c r="D275">
-        <v>4.0533420091295033E-3</v>
+        <v>3.4726078840088118E-3</v>
       </c>
       <c r="E275">
-        <v>1.1382655524311352E-3</v>
+        <v>6.9168895227530785E-4</v>
       </c>
       <c r="F275">
-        <v>2.239570483782532E-5</v>
+        <v>2.2761325449565115E-5</v>
       </c>
       <c r="G275">
-        <v>4.5261404599521648E-4</v>
+        <v>1.003946877521932E-3</v>
       </c>
       <c r="H275">
-        <v>1.8574846916962426E-3</v>
+        <v>2.798635738860215E-3</v>
       </c>
       <c r="I275">
-        <v>3.5541932981112455E-3</v>
+        <v>4.5014546370442466E-3</v>
       </c>
       <c r="J275">
-        <v>4.8975285967066641E-3</v>
-      </c>
-    </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.3900751809126939E-3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A276">
-        <v>9.9000000000000005E-2</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="B276">
         <v>36</v>
       </c>
       <c r="C276">
-        <v>9.2774371460456629E-3</v>
+        <v>8.7537746480221661E-3</v>
       </c>
       <c r="D276">
-        <v>3.4726078840088118E-3</v>
+        <v>2.4514596153664839E-3</v>
       </c>
       <c r="E276">
-        <v>6.9168895227530785E-4</v>
+        <v>1.396609100604215E-4</v>
       </c>
       <c r="F276">
-        <v>2.2761325449565115E-5</v>
+        <v>5.0536026890500324E-4</v>
       </c>
       <c r="G276">
-        <v>1.003946877521932E-3</v>
+        <v>2.4535683505868024E-3</v>
       </c>
       <c r="H276">
-        <v>2.798635738860215E-3</v>
+        <v>4.5014566900493571E-3</v>
       </c>
       <c r="I276">
-        <v>4.5014546370442466E-3</v>
+        <v>5.4307447206778997E-3</v>
       </c>
       <c r="J276">
-        <v>5.3900751809126939E-3</v>
-      </c>
-    </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4.7703695895321791E-3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A277">
-        <v>0.11700000000000001</v>
+        <v>0.126</v>
       </c>
       <c r="B277">
         <v>36</v>
       </c>
       <c r="C277">
-        <v>8.7537746480221661E-3</v>
+        <v>8.4978382521441569E-3</v>
       </c>
       <c r="D277">
-        <v>2.4514596153664839E-3</v>
+        <v>2.0105307194570126E-3</v>
       </c>
       <c r="E277">
-        <v>1.396609100604215E-4</v>
+        <v>2.3160563398035885E-5</v>
       </c>
       <c r="F277">
-        <v>5.0536026890500324E-4</v>
+        <v>9.3507598003429878E-4</v>
       </c>
       <c r="G277">
-        <v>2.4535683505868024E-3</v>
+        <v>3.2243095729190918E-3</v>
       </c>
       <c r="H277">
-        <v>4.5014566900493571E-3</v>
+        <v>5.0791106508547715E-3</v>
       </c>
       <c r="I277">
-        <v>5.4307447206778997E-3</v>
+        <v>5.2925010809506384E-3</v>
       </c>
       <c r="J277">
-        <v>4.7703695895321791E-3</v>
-      </c>
-    </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.8003339987376459E-3</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A278">
-        <v>0.126</v>
+        <v>0.153</v>
       </c>
       <c r="B278">
         <v>36</v>
       </c>
       <c r="C278">
-        <v>8.4978382521441569E-3</v>
+        <v>7.7537804482570851E-3</v>
       </c>
       <c r="D278">
-        <v>2.0105307194570126E-3</v>
+        <v>9.610309214367704E-4</v>
       </c>
       <c r="E278">
-        <v>2.3160563398035885E-5</v>
+        <v>2.2565594542113077E-4</v>
       </c>
       <c r="F278">
-        <v>9.3507598003429878E-4</v>
+        <v>2.6268831342880915E-3</v>
       </c>
       <c r="G278">
-        <v>3.2243095729190918E-3</v>
+        <v>5.0369064918967966E-3</v>
       </c>
       <c r="H278">
-        <v>5.0791106508547715E-3</v>
+        <v>5.1337125362755269E-3</v>
       </c>
       <c r="I278">
-        <v>5.2925010809506384E-3</v>
+        <v>2.9439983041634294E-3</v>
       </c>
       <c r="J278">
-        <v>3.8003339987376459E-3</v>
-      </c>
-    </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.4934850310076196E-4</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A279">
-        <v>0.153</v>
+        <v>0.18</v>
       </c>
       <c r="B279">
         <v>36</v>
       </c>
       <c r="C279">
-        <v>7.7537804482570851E-3</v>
+        <v>7.0456501865559483E-3</v>
       </c>
       <c r="D279">
-        <v>9.610309214367704E-4</v>
+        <v>3.0668239445489986E-4</v>
       </c>
       <c r="E279">
-        <v>2.2565594542113077E-4</v>
+        <v>1.0672834431458094E-3</v>
       </c>
       <c r="F279">
-        <v>2.6268831342880915E-3</v>
+        <v>4.3055037882942697E-3</v>
       </c>
       <c r="G279">
-        <v>5.0369064918967966E-3</v>
+        <v>5.3400519414024128E-3</v>
       </c>
       <c r="H279">
-        <v>5.1337125362755269E-3</v>
+        <v>3.0241811673848758E-3</v>
       </c>
       <c r="I279">
-        <v>2.9439983041634294E-3</v>
+        <v>3.3111807416285461E-4</v>
       </c>
       <c r="J279">
-        <v>5.4934850310076196E-4</v>
-      </c>
-    </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.3343775251774456E-4</v>
+      </c>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A280">
-        <v>0.18</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="B280">
         <v>36</v>
       </c>
       <c r="C280">
-        <v>7.0456501865559483E-3</v>
+        <v>6.5937058715284198E-3</v>
       </c>
       <c r="D280">
-        <v>3.0668239445489986E-4</v>
+        <v>7.6867349581732344E-5</v>
       </c>
       <c r="E280">
-        <v>1.0672834431458094E-3</v>
+        <v>1.8462470414564343E-3</v>
       </c>
       <c r="F280">
-        <v>4.3055037882942697E-3</v>
+        <v>5.0804687206640053E-3</v>
       </c>
       <c r="G280">
-        <v>5.3400519414024128E-3</v>
+        <v>4.6029857615280112E-3</v>
       </c>
       <c r="H280">
-        <v>3.0241811673848758E-3</v>
+        <v>1.3235966159629736E-3</v>
       </c>
       <c r="I280">
-        <v>3.3111807416285461E-4</v>
+        <v>1.024698080277861E-4</v>
       </c>
       <c r="J280">
-        <v>6.3343775251774456E-4</v>
-      </c>
-    </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.8720711251550546E-3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A281">
-        <v>0.19800000000000001</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="B281">
         <v>36</v>
       </c>
       <c r="C281">
-        <v>6.5937058715284198E-3</v>
+        <v>5.9462481138367468E-3</v>
       </c>
       <c r="D281">
-        <v>7.6867349581732344E-5</v>
+        <v>1.51872615599077E-5</v>
       </c>
       <c r="E281">
-        <v>1.8462470414564343E-3</v>
+        <v>3.1226742124929284E-3</v>
       </c>
       <c r="F281">
-        <v>5.0804687206640053E-3</v>
+        <v>5.4196050442628799E-3</v>
       </c>
       <c r="G281">
-        <v>4.6029857615280112E-3</v>
+        <v>2.6220028151313548E-3</v>
       </c>
       <c r="H281">
-        <v>1.3235966159629736E-3</v>
+        <v>3.8149043813780785E-6</v>
       </c>
       <c r="I281">
-        <v>1.024698080277861E-4</v>
+        <v>2.438258654714733E-3</v>
       </c>
       <c r="J281">
-        <v>2.8720711251550546E-3</v>
-      </c>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.0236711219256488E-3</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A282">
-        <v>0.22500000000000001</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="B282">
         <v>36</v>
       </c>
       <c r="C282">
-        <v>5.9462481138367468E-3</v>
+        <v>5.1402356432083502E-3</v>
       </c>
       <c r="D282">
-        <v>1.51872615599077E-5</v>
+        <v>3.9055390424839727E-4</v>
       </c>
       <c r="E282">
-        <v>3.1226742124929284E-3</v>
+        <v>4.5973397330777354E-3</v>
       </c>
       <c r="F282">
-        <v>5.4196050442628799E-3</v>
+        <v>4.2941812979494674E-3</v>
       </c>
       <c r="G282">
-        <v>2.6220028151313548E-3</v>
+        <v>2.9354892840755394E-4</v>
       </c>
       <c r="H282">
-        <v>3.8149043813780785E-6</v>
+        <v>1.9366014440944611E-3</v>
       </c>
       <c r="I282">
-        <v>2.438258654714733E-3</v>
+        <v>6.0853344001948768E-3</v>
       </c>
       <c r="J282">
-        <v>6.0236711219256488E-3</v>
-      </c>
-    </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.9438338609032939E-3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A283">
-        <v>0.26100000000000001</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="B283">
         <v>36</v>
       </c>
       <c r="C283">
-        <v>5.1402356432083502E-3</v>
+        <v>4.7618914551974074E-3</v>
       </c>
       <c r="D283">
-        <v>3.9055390424839727E-4</v>
+        <v>7.3894228584089709E-4</v>
       </c>
       <c r="E283">
-        <v>4.5973397330777354E-3</v>
+        <v>5.0873000429127813E-3</v>
       </c>
       <c r="F283">
-        <v>4.2941812979494674E-3</v>
+        <v>3.265242509376951E-3</v>
       </c>
       <c r="G283">
-        <v>2.9354892840755394E-4</v>
+        <v>5.973723346900063E-6</v>
       </c>
       <c r="H283">
-        <v>1.9366014440944611E-3</v>
+        <v>3.8326265452825448E-3</v>
       </c>
       <c r="I283">
-        <v>6.0853344001948768E-3</v>
+        <v>6.0020329511732608E-3</v>
       </c>
       <c r="J283">
-        <v>3.9438338609032939E-3</v>
-      </c>
-    </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.4077546832804921E-3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A284">
-        <v>0.27900000000000003</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="B284">
         <v>36</v>
       </c>
       <c r="C284">
-        <v>4.7618914551974074E-3</v>
+        <v>4.4000206447703371E-3</v>
       </c>
       <c r="D284">
-        <v>7.3894228584089709E-4</v>
+        <v>1.1710748436489814E-3</v>
       </c>
       <c r="E284">
-        <v>5.0873000429127813E-3</v>
+        <v>5.3533784388575568E-3</v>
       </c>
       <c r="F284">
-        <v>3.265242509376951E-3</v>
+        <v>2.1457136129249448E-3</v>
       </c>
       <c r="G284">
-        <v>5.973723346900063E-6</v>
+        <v>4.8418477600539864E-4</v>
       </c>
       <c r="H284">
-        <v>3.8326265452825448E-3</v>
+        <v>5.4695057798868716E-3</v>
       </c>
       <c r="I284">
-        <v>6.0020329511732608E-3</v>
+        <v>4.4406139716006909E-3</v>
       </c>
       <c r="J284">
-        <v>1.4077546832804921E-3</v>
-      </c>
-    </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.158291254261377E-5</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A285">
-        <v>0.29699999999999999</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="B285">
         <v>36</v>
       </c>
       <c r="C285">
-        <v>4.4000206447703371E-3</v>
+        <v>3.7256446159771371E-3</v>
       </c>
       <c r="D285">
-        <v>1.1710748436489814E-3</v>
+        <v>2.2114419898378473E-3</v>
       </c>
       <c r="E285">
-        <v>5.3533784388575568E-3</v>
+        <v>5.1578286686436887E-3</v>
       </c>
       <c r="F285">
-        <v>2.1457136129249448E-3</v>
+        <v>3.7212480315748344E-4</v>
       </c>
       <c r="G285">
-        <v>4.8418477600539864E-4</v>
+        <v>3.1359206014311518E-3</v>
       </c>
       <c r="H285">
-        <v>5.4695057798868716E-3</v>
+        <v>5.8454066552080276E-3</v>
       </c>
       <c r="I285">
-        <v>4.4406139716006909E-3</v>
+        <v>4.4049060459541348E-4</v>
       </c>
       <c r="J285">
-        <v>3.158291254261377E-5</v>
-      </c>
-    </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.0573783545318647E-3</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A286">
-        <v>0.33300000000000002</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="B286">
         <v>36</v>
       </c>
       <c r="C286">
-        <v>3.7256446159771371E-3</v>
+        <v>3.4130417592925038E-3</v>
       </c>
       <c r="D286">
-        <v>2.2114419898378473E-3</v>
+        <v>2.7813570729809814E-3</v>
       </c>
       <c r="E286">
-        <v>5.1578286686436887E-3</v>
+        <v>4.7203827379271304E-3</v>
       </c>
       <c r="F286">
-        <v>3.7212480315748344E-4</v>
+        <v>1.7560613755081105E-5</v>
       </c>
       <c r="G286">
-        <v>3.1359206014311518E-3</v>
+        <v>4.6514868947815386E-3</v>
       </c>
       <c r="H286">
-        <v>5.8454066552080276E-3</v>
+        <v>4.4405103060187303E-3</v>
       </c>
       <c r="I286">
-        <v>4.4049060459541348E-4</v>
+        <v>6.001793578801452E-5</v>
       </c>
       <c r="J286">
-        <v>3.0573783545318647E-3</v>
-      </c>
-    </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.4057538599859758E-3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A287">
-        <v>0.35099999999999998</v>
+        <v>0.378</v>
       </c>
       <c r="B287">
         <v>36</v>
       </c>
       <c r="C287">
-        <v>3.4130417592925038E-3</v>
+        <v>2.9746134694505167E-3</v>
       </c>
       <c r="D287">
-        <v>2.7813570729809814E-3</v>
+        <v>3.645352123522864E-3</v>
       </c>
       <c r="E287">
-        <v>4.7203827379271304E-3</v>
+        <v>3.7463045818737989E-3</v>
       </c>
       <c r="F287">
-        <v>1.7560613755081105E-5</v>
+        <v>3.5115981701322121E-4</v>
       </c>
       <c r="G287">
-        <v>4.6514868947815386E-3</v>
+        <v>6.1139647177862457E-3</v>
       </c>
       <c r="H287">
-        <v>4.4405103060187303E-3</v>
+        <v>1.6346431890004736E-3</v>
       </c>
       <c r="I287">
-        <v>6.001793578801452E-5</v>
+        <v>2.2765417861715614E-3</v>
       </c>
       <c r="J287">
-        <v>5.4057538599859758E-3</v>
-      </c>
-    </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.7831959559528833E-3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A288">
-        <v>0.378</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="B288">
         <v>36</v>
       </c>
       <c r="C288">
-        <v>2.9746134694505167E-3</v>
+        <v>2.7024475277394547E-3</v>
       </c>
       <c r="D288">
-        <v>3.645352123522864E-3</v>
+        <v>4.2014148477648684E-3</v>
       </c>
       <c r="E288">
-        <v>3.7463045818737989E-3</v>
+        <v>2.9693082998175895E-3</v>
       </c>
       <c r="F288">
-        <v>3.5115981701322121E-4</v>
+        <v>1.1100817159477863E-3</v>
       </c>
       <c r="G288">
-        <v>6.1139647177862457E-3</v>
+        <v>6.1887722230313212E-3</v>
       </c>
       <c r="H288">
-        <v>1.6346431890004736E-3</v>
+        <v>3.1476204376981596E-4</v>
       </c>
       <c r="I288">
-        <v>2.2765417861715614E-3</v>
+        <v>4.5001381426733383E-3</v>
       </c>
       <c r="J288">
-        <v>5.7831959559528833E-3</v>
-      </c>
-    </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.6905235951957879E-3</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A289">
-        <v>0.39600000000000002</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="B289">
         <v>36</v>
       </c>
       <c r="C289">
-        <v>2.7024475277394547E-3</v>
+        <v>2.4461742271764397E-3</v>
       </c>
       <c r="D289">
-        <v>4.2014148477648684E-3</v>
+        <v>4.7223514959647316E-3</v>
       </c>
       <c r="E289">
-        <v>2.9693082998175895E-3</v>
+        <v>2.1687157697954144E-3</v>
       </c>
       <c r="F289">
-        <v>1.1100817159477863E-3</v>
+        <v>2.1758565519361564E-3</v>
       </c>
       <c r="G289">
-        <v>6.1887722230313212E-3</v>
+        <v>5.4918607542441848E-3</v>
       </c>
       <c r="H289">
-        <v>3.1476204376981596E-4</v>
+        <v>4.4074161288416649E-5</v>
       </c>
       <c r="I289">
-        <v>4.5001381426733383E-3</v>
+        <v>6.0041794072945463E-3</v>
       </c>
       <c r="J289">
-        <v>3.6905235951957879E-3</v>
-      </c>
-    </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.203106291139926E-3</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A290">
-        <v>0.41399999999999998</v>
+        <v>0.432</v>
       </c>
       <c r="B290">
         <v>36</v>
       </c>
       <c r="C290">
-        <v>2.4461742271764397E-3</v>
+        <v>2.2055800030765542E-3</v>
       </c>
       <c r="D290">
-        <v>4.7223514959647316E-3</v>
+        <v>5.1935601165409503E-3</v>
       </c>
       <c r="E290">
-        <v>2.1687157697954144E-3</v>
+        <v>1.4144855620566255E-3</v>
       </c>
       <c r="F290">
-        <v>2.1758565519361564E-3</v>
+        <v>3.3863209005395704E-3</v>
       </c>
       <c r="G290">
-        <v>5.4918607542441848E-3</v>
+        <v>4.1984001487362765E-3</v>
       </c>
       <c r="H290">
-        <v>4.4074161288416649E-5</v>
+        <v>9.2259055544402578E-4</v>
       </c>
       <c r="I290">
-        <v>6.0041794072945463E-3</v>
+        <v>6.0117396438539973E-3</v>
       </c>
       <c r="J290">
-        <v>1.203106291139926E-3</v>
-      </c>
-    </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.1242476706838208E-6</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A291">
-        <v>0.432</v>
+        <v>0.441</v>
       </c>
       <c r="B291">
         <v>36</v>
       </c>
       <c r="C291">
-        <v>2.2055800030765542E-3</v>
+        <v>2.0910860219302218E-3</v>
       </c>
       <c r="D291">
-        <v>5.1935601165409503E-3</v>
+        <v>5.4064855899634877E-3</v>
       </c>
       <c r="E291">
-        <v>1.4144855620566255E-3</v>
+        <v>1.0757251531833048E-3</v>
       </c>
       <c r="F291">
-        <v>3.3863209005395704E-3</v>
+        <v>3.9878702529615728E-3</v>
       </c>
       <c r="G291">
-        <v>4.1984001487362765E-3</v>
+        <v>3.4260786462019057E-3</v>
       </c>
       <c r="H291">
-        <v>9.2259055544402578E-4</v>
+        <v>1.7040787675821267E-3</v>
       </c>
       <c r="I291">
-        <v>6.0117396438539973E-3</v>
+        <v>5.419854559714562E-3</v>
       </c>
       <c r="J291">
-        <v>6.1242476706838208E-6</v>
-      </c>
-    </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.0072463326341122E-4</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A292">
-        <v>0.441</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="B292">
         <v>36</v>
       </c>
       <c r="C292">
-        <v>2.0910860219302218E-3</v>
+        <v>1.7703951200036989E-3</v>
       </c>
       <c r="D292">
-        <v>5.4064855899634877E-3</v>
+        <v>5.9385084460451603E-3</v>
       </c>
       <c r="E292">
-        <v>1.0757251531833048E-3</v>
+        <v>3.0061658925296426E-4</v>
       </c>
       <c r="F292">
-        <v>3.9878702529615728E-3</v>
+        <v>5.5032633751653662E-3</v>
       </c>
       <c r="G292">
-        <v>3.4260786462019057E-3</v>
+        <v>1.1951656942226704E-3</v>
       </c>
       <c r="H292">
-        <v>1.7040787675821267E-3</v>
+        <v>4.5009322278625405E-3</v>
       </c>
       <c r="I292">
-        <v>5.419854559714562E-3</v>
+        <v>2.2972834769960666E-3</v>
       </c>
       <c r="J292">
-        <v>2.0072463326341122E-4</v>
-      </c>
-    </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.3038907112402992E-3</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A293">
-        <v>0.46800000000000003</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="B293">
         <v>36</v>
       </c>
       <c r="C293">
-        <v>1.7703951200036989E-3</v>
+        <v>1.5751972736934422E-3</v>
       </c>
       <c r="D293">
-        <v>5.9385084460451603E-3</v>
+        <v>6.1938739406483933E-3</v>
       </c>
       <c r="E293">
-        <v>3.0061658925296426E-4</v>
+        <v>4.149106138560935E-5</v>
       </c>
       <c r="F293">
-        <v>5.5032633751653662E-3</v>
+        <v>6.0822803184238782E-3</v>
       </c>
       <c r="G293">
-        <v>1.1951656942226704E-3</v>
+        <v>2.4339253121190979E-4</v>
       </c>
       <c r="H293">
-        <v>4.5009322278625405E-3</v>
+        <v>5.8597298438472552E-3</v>
       </c>
       <c r="I293">
-        <v>2.2972834769960666E-3</v>
+        <v>4.9425335755449095E-4</v>
       </c>
       <c r="J293">
-        <v>3.3038907112402992E-3</v>
-      </c>
-    </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.5649533047252191E-3</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A294">
-        <v>0.48599999999999999</v>
+        <v>0.495</v>
       </c>
       <c r="B294">
         <v>36</v>
       </c>
       <c r="C294">
-        <v>1.5751972736934422E-3</v>
+        <v>1.4830464364319941E-3</v>
       </c>
       <c r="D294">
-        <v>6.1938739406483933E-3</v>
+        <v>6.2894875068881971E-3</v>
       </c>
       <c r="E294">
-        <v>4.149106138560935E-5</v>
+        <v>8.0583197972772459E-7</v>
       </c>
       <c r="F294">
-        <v>6.0822803184238782E-3</v>
+        <v>6.2026320173810571E-3</v>
       </c>
       <c r="G294">
-        <v>2.4339253121190979E-4</v>
+        <v>3.208196059563966E-5</v>
       </c>
       <c r="H294">
-        <v>5.8597298438472552E-3</v>
+        <v>6.1706830496927731E-3</v>
       </c>
       <c r="I294">
-        <v>4.9425335755449095E-4</v>
+        <v>6.4522274885134352E-5</v>
       </c>
       <c r="J294">
-        <v>5.5649533047252191E-3</v>
-      </c>
-    </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.1313643220436915E-3</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A295">
-        <v>0.495</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="B295">
         <v>36</v>
       </c>
       <c r="C295">
-        <v>1.4830464364319941E-3</v>
+        <v>1.2278034225057725E-3</v>
       </c>
       <c r="D295">
-        <v>6.2894875068881971E-3</v>
+        <v>6.4433593604730334E-3</v>
       </c>
       <c r="E295">
-        <v>8.0583197972772459E-7</v>
+        <v>2.4903352067304988E-4</v>
       </c>
       <c r="F295">
-        <v>6.2026320173810571E-3</v>
+        <v>5.8435986578944249E-3</v>
       </c>
       <c r="G295">
-        <v>3.208196059563966E-5</v>
+        <v>5.7746576367094179E-4</v>
       </c>
       <c r="H295">
-        <v>6.1706830496927731E-3</v>
+        <v>5.3624186930204864E-3</v>
       </c>
       <c r="I295">
-        <v>6.4522274885134352E-5</v>
+        <v>1.1729187774250978E-3</v>
       </c>
       <c r="J295">
-        <v>6.1313643220436915E-3</v>
-      </c>
-    </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4.6909760054359203E-3</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A296">
-        <v>0.52200000000000002</v>
+        <v>0.55800000000000005</v>
       </c>
       <c r="B296">
         <v>36</v>
       </c>
       <c r="C296">
-        <v>1.2278034225057725E-3</v>
+        <v>9.3495427518471431E-4</v>
       </c>
       <c r="D296">
-        <v>6.4433593604730334E-3</v>
+        <v>6.3388189426139595E-3</v>
       </c>
       <c r="E296">
-        <v>2.4903352067304988E-4</v>
+        <v>1.37684404189635E-3</v>
       </c>
       <c r="F296">
-        <v>5.8435986578944249E-3</v>
+        <v>3.9741271102426631E-3</v>
       </c>
       <c r="G296">
-        <v>5.7746576367094179E-4</v>
+        <v>3.308475267823332E-3</v>
       </c>
       <c r="H296">
-        <v>5.3624186930204864E-3</v>
+        <v>1.8047108852732867E-3</v>
       </c>
       <c r="I296">
-        <v>1.1729187774250978E-3</v>
+        <v>5.3352655912077733E-3</v>
       </c>
       <c r="J296">
-        <v>4.6909760054359203E-3</v>
-      </c>
-    </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.5562087666641082E-4</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A297">
-        <v>0.55800000000000005</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="B297">
         <v>36</v>
       </c>
       <c r="C297">
-        <v>9.3495427518471431E-4</v>
+        <v>8.0781237989917395E-4</v>
       </c>
       <c r="D297">
-        <v>6.3388189426139595E-3</v>
+        <v>6.1610624872792483E-3</v>
       </c>
       <c r="E297">
-        <v>1.37684404189635E-3</v>
+        <v>2.2000715314677197E-3</v>
       </c>
       <c r="F297">
-        <v>3.9741271102426631E-3</v>
+        <v>2.7516938452650688E-3</v>
       </c>
       <c r="G297">
-        <v>3.308475267823332E-3</v>
+        <v>4.7856449827715164E-3</v>
       </c>
       <c r="H297">
-        <v>1.8047108852732867E-3</v>
+        <v>4.0491904864079788E-4</v>
       </c>
       <c r="I297">
-        <v>5.3352655912077733E-3</v>
+        <v>6.2166273472273829E-3</v>
       </c>
       <c r="J297">
-        <v>2.5562087666641082E-4</v>
-      </c>
-    </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.9594067105301341E-4</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A298">
-        <v>0.57599999999999996</v>
+        <v>0.621</v>
       </c>
       <c r="B298">
         <v>36</v>
       </c>
       <c r="C298">
-        <v>8.0781237989917395E-4</v>
+        <v>5.4197857711310582E-4</v>
       </c>
       <c r="D298">
-        <v>6.1610624872792483E-3</v>
+        <v>5.4072225651837311E-3</v>
       </c>
       <c r="E298">
-        <v>2.2000715314677197E-3</v>
+        <v>4.5422012454751732E-3</v>
       </c>
       <c r="F298">
-        <v>2.7516938452650688E-3</v>
+        <v>3.2275197087267747E-4</v>
       </c>
       <c r="G298">
-        <v>4.7856449827715164E-3</v>
+        <v>6.0542315913758816E-3</v>
       </c>
       <c r="H298">
-        <v>4.0491904864079788E-4</v>
+        <v>1.5284620429941069E-3</v>
       </c>
       <c r="I298">
-        <v>6.2166273472273829E-3</v>
+        <v>2.4043317260639442E-3</v>
       </c>
       <c r="J298">
-        <v>2.9594067105301341E-4</v>
-      </c>
-    </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.7079374627017022E-3</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A299">
-        <v>0.60299999999999998</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="B299">
         <v>36</v>
       </c>
       <c r="C299">
-        <v>6.3974288537250546E-4</v>
+        <v>4.1528278744694923E-4</v>
       </c>
       <c r="D299">
-        <v>5.7560805708792243E-3</v>
+        <v>4.7929388840282153E-3</v>
       </c>
       <c r="E299">
-        <v>3.5987062167768952E-3</v>
+        <v>5.8054592442381018E-3</v>
       </c>
       <c r="F299">
-        <v>1.0775486015012559E-3</v>
+        <v>3.1066318563870152E-5</v>
       </c>
       <c r="G299">
-        <v>6.1022522891378862E-3</v>
+        <v>4.6209375518087674E-3</v>
       </c>
       <c r="H299">
-        <v>2.6557531378620757E-4</v>
+        <v>4.3086222587245754E-3</v>
       </c>
       <c r="I299">
-        <v>4.6170788847058721E-3</v>
+        <v>8.898133331110038E-5</v>
       </c>
       <c r="J299">
-        <v>3.5471960972285254E-3</v>
-      </c>
-    </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.5059226855212456E-3</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A300">
-        <v>0.621</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="B300">
         <v>36</v>
       </c>
       <c r="C300">
-        <v>5.4197857711310582E-4</v>
+        <v>3.1067331732189752E-4</v>
       </c>
       <c r="D300">
-        <v>5.4072225651837311E-3</v>
+        <v>4.1059594400874528E-3</v>
       </c>
       <c r="E300">
-        <v>4.5422012454751732E-3</v>
+        <v>6.7115037818651097E-3</v>
       </c>
       <c r="F300">
-        <v>3.2275197087267747E-4</v>
+        <v>8.3071277398583576E-4</v>
       </c>
       <c r="G300">
-        <v>6.0542315913758816E-3</v>
+        <v>2.3278421770083469E-3</v>
       </c>
       <c r="H300">
-        <v>1.5284620429941069E-3</v>
+        <v>6.0996767635234988E-3</v>
       </c>
       <c r="I300">
-        <v>2.4043317260639442E-3</v>
+        <v>1.0849061005313448E-3</v>
       </c>
       <c r="J300">
-        <v>5.7079374627017022E-3</v>
-      </c>
-    </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.9213141318166337E-3</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A301">
-        <v>0.64800000000000002</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="B301">
         <v>36</v>
       </c>
       <c r="C301">
-        <v>4.1528278744694923E-4</v>
+        <v>2.8033948422193805E-4</v>
       </c>
       <c r="D301">
-        <v>4.7929388840282153E-3</v>
+        <v>3.8681750360842031E-3</v>
       </c>
       <c r="E301">
-        <v>5.8054592442381018E-3</v>
+        <v>6.9081026842395471E-3</v>
       </c>
       <c r="F301">
-        <v>3.1066318563870152E-5</v>
+        <v>1.3077820408206816E-3</v>
       </c>
       <c r="G301">
-        <v>4.6209375518087674E-3</v>
+        <v>1.5935902801991898E-3</v>
       </c>
       <c r="H301">
-        <v>4.3086222587245754E-3</v>
+        <v>6.1711605029354764E-3</v>
       </c>
       <c r="I301">
-        <v>8.898133331110038E-5</v>
+        <v>2.0660093872620568E-3</v>
       </c>
       <c r="J301">
-        <v>5.5059226855212456E-3</v>
-      </c>
-    </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.4442731221760379E-4</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A302">
-        <v>0.67500000000000004</v>
+        <v>0.69299999999999995</v>
       </c>
       <c r="B302">
         <v>36</v>
       </c>
       <c r="C302">
-        <v>3.1067331732189752E-4</v>
+        <v>2.5213782970049509E-4</v>
       </c>
       <c r="D302">
-        <v>4.1059594400874528E-3</v>
+        <v>3.6286203899811974E-3</v>
       </c>
       <c r="E302">
-        <v>6.7115037818651097E-3</v>
+        <v>7.0459522003458617E-3</v>
       </c>
       <c r="F302">
-        <v>8.3071277398583576E-4</v>
+        <v>1.864842672273828E-3</v>
       </c>
       <c r="G302">
-        <v>2.3278421770083469E-3</v>
+        <v>9.5639710786580103E-4</v>
       </c>
       <c r="H302">
-        <v>6.0996767635234988E-3</v>
+        <v>5.945285859829205E-3</v>
       </c>
       <c r="I302">
-        <v>1.0849061005313448E-3</v>
+        <v>3.1845674051008853E-3</v>
       </c>
       <c r="J302">
-        <v>1.9213141318166337E-3</v>
-      </c>
-    </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.6864516804284397E-4</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A303">
-        <v>0.68400000000000005</v>
+        <v>0.72</v>
       </c>
       <c r="B303">
         <v>36</v>
       </c>
       <c r="C303">
-        <v>2.8033948422193805E-4</v>
+        <v>1.7949860210638856E-4</v>
       </c>
       <c r="D303">
-        <v>3.8681750360842031E-3</v>
+        <v>2.9144822621971185E-3</v>
       </c>
       <c r="E303">
-        <v>6.9081026842395471E-3</v>
+        <v>7.0931702536027102E-3</v>
       </c>
       <c r="F303">
-        <v>1.3077820408206816E-3</v>
+        <v>3.8058809978472846E-3</v>
       </c>
       <c r="G303">
-        <v>1.5935902801991898E-3</v>
+        <v>1.9882216457316716E-6</v>
       </c>
       <c r="H303">
-        <v>6.1711605029354764E-3</v>
+        <v>3.8268868883388203E-3</v>
       </c>
       <c r="I303">
-        <v>2.0660093872620568E-3</v>
+        <v>5.8932064149941499E-3</v>
       </c>
       <c r="J303">
-        <v>8.4442731221760379E-4</v>
-      </c>
-    </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.2759772125415336E-3</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A304">
-        <v>0.69299999999999995</v>
+        <v>0.747</v>
       </c>
       <c r="B304">
         <v>36</v>
       </c>
       <c r="C304">
-        <v>2.5213782970049509E-4</v>
+        <v>1.23056209084159E-4</v>
       </c>
       <c r="D304">
-        <v>3.6286203899811974E-3</v>
+        <v>2.2365257441041399E-3</v>
       </c>
       <c r="E304">
-        <v>7.0459522003458617E-3</v>
+        <v>6.6099049202129655E-3</v>
       </c>
       <c r="F304">
-        <v>1.864842672273828E-3</v>
+        <v>5.6627090748208736E-3</v>
       </c>
       <c r="G304">
-        <v>9.5639710786580103E-4</v>
+        <v>8.1906914543786581E-4</v>
       </c>
       <c r="H304">
-        <v>5.945285859829205E-3</v>
+        <v>1.1025177597153682E-3</v>
       </c>
       <c r="I304">
-        <v>3.1845674051008853E-3</v>
+        <v>5.5115801534774064E-3</v>
       </c>
       <c r="J304">
-        <v>1.6864516804284397E-4</v>
-      </c>
-    </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4.9548483145002153E-3</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A305">
-        <v>0.72</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="B305">
         <v>36</v>
       </c>
       <c r="C305">
-        <v>1.7949860210638856E-4</v>
+        <v>6.9100507428401773E-5</v>
       </c>
       <c r="D305">
-        <v>2.9144822621971185E-3</v>
+        <v>1.4434355903243459E-3</v>
       </c>
       <c r="E305">
-        <v>7.0931702536027102E-3</v>
+        <v>5.3145662210012587E-3</v>
       </c>
       <c r="F305">
-        <v>3.8058809978472846E-3</v>
+        <v>7.0450345184333131E-3</v>
       </c>
       <c r="G305">
-        <v>1.9882216457316716E-6</v>
+        <v>3.8825940746148565E-3</v>
       </c>
       <c r="H305">
-        <v>3.8268868883388203E-3</v>
+        <v>2.3208074949340239E-4</v>
       </c>
       <c r="I305">
-        <v>5.8932064149941499E-3</v>
+        <v>1.4010826696440959E-3</v>
       </c>
       <c r="J305">
-        <v>1.2759772125415336E-3</v>
-      </c>
-    </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.2920722568194373E-3</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A306">
-        <v>0.747</v>
+        <v>0.81</v>
       </c>
       <c r="B306">
         <v>36</v>
       </c>
       <c r="C306">
-        <v>1.23056209084159E-4</v>
+        <v>4.1734612773149277E-5</v>
       </c>
       <c r="D306">
-        <v>2.2365257441041399E-3</v>
+        <v>9.6034734634250574E-4</v>
       </c>
       <c r="E306">
-        <v>6.6099049202129655E-3</v>
+        <v>4.0705891656203546E-3</v>
       </c>
       <c r="F306">
-        <v>5.6627090748208736E-3</v>
+        <v>6.8808574387804466E-3</v>
       </c>
       <c r="G306">
-        <v>8.1906914543786581E-4</v>
+        <v>6.1463268893473212E-3</v>
       </c>
       <c r="H306">
-        <v>1.1025177597153682E-3</v>
+        <v>2.4437700353025314E-3</v>
       </c>
       <c r="I306">
-        <v>5.5115801534774064E-3</v>
+        <v>2.3676463270526435E-5</v>
       </c>
       <c r="J306">
-        <v>4.9548483145002153E-3</v>
-      </c>
-    </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.6455070863988308E-3</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A307">
-        <v>0.78300000000000003</v>
+        <v>0.83699999999999997</v>
       </c>
       <c r="B307">
         <v>36</v>
       </c>
       <c r="C307">
-        <v>6.9100507428401773E-5</v>
+        <v>2.3223221107871247E-5</v>
       </c>
       <c r="D307">
-        <v>1.4434355903243459E-3</v>
+        <v>5.8514951648594427E-4</v>
       </c>
       <c r="E307">
-        <v>5.3145662210012587E-3</v>
+        <v>2.8066945349864789E-3</v>
       </c>
       <c r="F307">
-        <v>7.0450345184333131E-3</v>
+        <v>5.7646034702098061E-3</v>
       </c>
       <c r="G307">
-        <v>3.8825940746148565E-3</v>
+        <v>7.1080973960687367E-3</v>
       </c>
       <c r="H307">
-        <v>2.3208074949340239E-4</v>
+        <v>5.4730254265368105E-3</v>
       </c>
       <c r="I307">
-        <v>1.4010826696440959E-3</v>
+        <v>2.1549055860631385E-3</v>
       </c>
       <c r="J307">
-        <v>5.2920722568194373E-3</v>
-      </c>
-    </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.4019761951644274E-5</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A308">
-        <v>0.81</v>
+        <v>0.873</v>
       </c>
       <c r="B308">
         <v>36</v>
       </c>
       <c r="C308">
-        <v>4.1734612773149277E-5</v>
+        <v>8.8663206373711236E-6</v>
       </c>
       <c r="D308">
-        <v>9.6034734634250574E-4</v>
+        <v>2.4999022052137304E-4</v>
       </c>
       <c r="E308">
-        <v>4.0705891656203546E-3</v>
+        <v>1.3822688382815794E-3</v>
       </c>
       <c r="F308">
-        <v>6.8808574387804466E-3</v>
+        <v>3.4849734306319721E-3</v>
       </c>
       <c r="G308">
-        <v>6.1463268893473212E-3</v>
+        <v>5.7808491776367363E-3</v>
       </c>
       <c r="H308">
-        <v>2.4437700353025314E-3</v>
+        <v>7.0614140579516012E-3</v>
       </c>
       <c r="I308">
-        <v>2.3676463270526435E-5</v>
+        <v>6.5303304051190364E-3</v>
       </c>
       <c r="J308">
-        <v>1.6455070863988308E-3</v>
-      </c>
-    </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4.3853145076318588E-3</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A309">
-        <v>0.83699999999999997</v>
+        <v>0.90900000000000003</v>
       </c>
       <c r="B309">
         <v>36</v>
       </c>
       <c r="C309">
-        <v>2.3223221107871247E-5</v>
+        <v>2.4198670335745438E-6</v>
       </c>
       <c r="D309">
-        <v>5.8514951648594427E-4</v>
+        <v>7.5673338657352018E-5</v>
       </c>
       <c r="E309">
-        <v>2.8066945349864789E-3</v>
+        <v>4.7187855633788799E-4</v>
       </c>
       <c r="F309">
-        <v>5.7646034702098061E-3</v>
+        <v>1.3939606874920263E-3</v>
       </c>
       <c r="G309">
-        <v>7.1080973960687367E-3</v>
+        <v>2.838687688043076E-3</v>
       </c>
       <c r="H309">
-        <v>5.4730254265368105E-3</v>
+        <v>4.5447370025972133E-3</v>
       </c>
       <c r="I309">
-        <v>2.1549055860631385E-3</v>
+        <v>6.0792091933391827E-3</v>
       </c>
       <c r="J309">
-        <v>6.4019761951644274E-5</v>
-      </c>
-    </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.9916388845835415E-3</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A310">
-        <v>0.873</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="B310">
         <v>36</v>
       </c>
       <c r="C310">
-        <v>8.8663206373711236E-6</v>
+        <v>1.0194607828460374E-6</v>
       </c>
       <c r="D310">
-        <v>2.4999022052137304E-4</v>
+        <v>3.3471835428197282E-5</v>
       </c>
       <c r="E310">
-        <v>1.3822688382815794E-3</v>
+        <v>2.2009048867100599E-4</v>
       </c>
       <c r="F310">
-        <v>3.4849734306319721E-3</v>
+        <v>6.9418019709690734E-4</v>
       </c>
       <c r="G310">
-        <v>5.7808491776367363E-3</v>
+        <v>1.5298975136479539E-3</v>
       </c>
       <c r="H310">
-        <v>7.0614140579516012E-3</v>
+        <v>2.6958333489634067E-3</v>
       </c>
       <c r="I310">
-        <v>6.5303304051190364E-3</v>
+        <v>4.0540532924466842E-3</v>
       </c>
       <c r="J310">
-        <v>4.3853145076318588E-3</v>
-      </c>
-    </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.3887693267850329E-3</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A311">
-        <v>0.90900000000000003</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="B311">
         <v>36</v>
       </c>
       <c r="C311">
-        <v>2.4198670335745438E-6</v>
+        <v>3.3413373197985292E-7</v>
       </c>
       <c r="D311">
-        <v>7.5673338657352018E-5</v>
+        <v>1.1496399637853754E-5</v>
       </c>
       <c r="E311">
-        <v>4.7187855633788799E-4</v>
+        <v>7.9377987263388157E-5</v>
       </c>
       <c r="F311">
-        <v>1.3939606874920263E-3</v>
+        <v>2.652808362141195E-4</v>
       </c>
       <c r="G311">
-        <v>2.838687688043076E-3</v>
+        <v>6.2510164929969483E-4</v>
       </c>
       <c r="H311">
-        <v>4.5447370025972133E-3</v>
+        <v>1.1903651326183099E-3</v>
       </c>
       <c r="I311">
-        <v>6.0792091933391827E-3</v>
+        <v>1.9590278294418428E-3</v>
       </c>
       <c r="J311">
-        <v>6.9916388845835415E-3</v>
-      </c>
-    </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.8928150367626788E-3</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A312">
-        <v>0.92700000000000005</v>
+        <v>0.98099999999999998</v>
       </c>
       <c r="B312">
         <v>36</v>
       </c>
       <c r="C312">
-        <v>1.0194607828460374E-6</v>
+        <v>4.9213179139354219E-9</v>
       </c>
       <c r="D312">
-        <v>3.3471835428197282E-5</v>
+        <v>1.849630889213609E-7</v>
       </c>
       <c r="E312">
-        <v>2.2009048867100599E-4</v>
+        <v>1.3926219939728583E-6</v>
       </c>
       <c r="F312">
-        <v>6.9418019709690734E-4</v>
+        <v>5.1257847381863333E-6</v>
       </c>
       <c r="G312">
-        <v>1.5298975136479539E-3</v>
+        <v>1.3414475127553028E-5</v>
       </c>
       <c r="H312">
-        <v>2.6958333489634067E-3</v>
+        <v>2.8641708347793936E-5</v>
       </c>
       <c r="I312">
-        <v>4.0540532924466842E-3</v>
+        <v>5.3407645077557132E-5</v>
       </c>
       <c r="J312">
-        <v>5.3887693267850329E-3</v>
-      </c>
-    </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9.0399500930973689E-5</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A313">
-        <v>0.94499999999999995</v>
+        <v>0.999</v>
       </c>
       <c r="B313">
         <v>36</v>
       </c>
       <c r="C313">
-        <v>3.3413373197985292E-7</v>
+        <v>3.8400257057012698E-14</v>
       </c>
       <c r="D313">
-        <v>1.1496399637853754E-5</v>
+        <v>1.5046572694145843E-12</v>
       </c>
       <c r="E313">
-        <v>7.9377987263388157E-5</v>
+        <v>1.177389300734342E-11</v>
       </c>
       <c r="F313">
-        <v>2.652808362141195E-4</v>
+        <v>4.5119091679177244E-11</v>
       </c>
       <c r="G313">
-        <v>6.2510164929969483E-4</v>
+        <v>1.2301605514391832E-10</v>
       </c>
       <c r="H313">
-        <v>1.1903651326183099E-3</v>
+        <v>2.7393780866288146E-10</v>
       </c>
       <c r="I313">
-        <v>1.9590278294418428E-3</v>
+        <v>5.3314766076847062E-10</v>
       </c>
       <c r="J313">
-        <v>2.8928150367626788E-3</v>
-      </c>
-    </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A314">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="B314">
-        <v>36</v>
-      </c>
-      <c r="C314">
-        <v>4.9213179139354219E-9</v>
-      </c>
-      <c r="D314">
-        <v>1.849630889213609E-7</v>
-      </c>
-      <c r="E314">
-        <v>1.3926219939728583E-6</v>
-      </c>
-      <c r="F314">
-        <v>5.1257847381863333E-6</v>
-      </c>
-      <c r="G314">
-        <v>1.3414475127553028E-5</v>
-      </c>
-      <c r="H314">
-        <v>2.8641708347793936E-5</v>
-      </c>
-      <c r="I314">
-        <v>5.3407645077557132E-5</v>
-      </c>
-      <c r="J314">
-        <v>9.0399500930973689E-5</v>
-      </c>
-    </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A315">
-        <v>0.999</v>
-      </c>
-      <c r="B315">
-        <v>36</v>
-      </c>
-      <c r="C315">
-        <v>3.8400257057012698E-14</v>
-      </c>
-      <c r="D315">
-        <v>1.5046572694145843E-12</v>
-      </c>
-      <c r="E315">
-        <v>1.177389300734342E-11</v>
-      </c>
-      <c r="F315">
-        <v>4.5119091679177244E-11</v>
-      </c>
-      <c r="G315">
-        <v>1.2301605514391832E-10</v>
-      </c>
-      <c r="H315">
-        <v>2.7393780866288146E-10</v>
-      </c>
-      <c r="I315">
-        <v>5.3314766076847062E-10</v>
-      </c>
-      <c r="J315">
         <v>9.4128140678622191E-10</v>
       </c>
     </row>

</xml_diff>